<commit_message>
constraint to EU profiles for observations
</commit_message>
<xml_diff>
--- a/StructureDefinition-VunsEfr.xlsx
+++ b/StructureDefinition-VunsEfr.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-14T13:33:24+02:00</t>
+    <t>2025-05-23T16:57:29+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>EFR observation</t>
+    <t>Profile pour les épreuves fonctionnelles respiratoires</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>

<commit_message>
found a way to get rid of the lab patient
</commit_message>
<xml_diff>
--- a/StructureDefinition-VunsEfr.xlsx
+++ b/StructureDefinition-VunsEfr.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$67</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2826" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2433" uniqueCount="483">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-23T16:57:29+02:00</t>
+    <t>2025-05-27T16:55:56+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -825,198 +825,31 @@
 </t>
   </si>
   <si>
-    <t>Code defined by a terminology system</t>
+    <t>A reference to a code defined by a terminology system</t>
   </si>
   <si>
     <t>A reference to a code defined by a terminology system.</t>
   </si>
   <si>
-    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
+    <t>Codes may be defined very casually in enumerations or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.</t>
   </si>
   <si>
     <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
   </si>
   <si>
+    <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
+  &lt;system value="http://snomed.info/sct"/&gt;
+  &lt;code value="23426006"/&gt;
+&lt;/valueCoding&gt;</t>
+  </si>
+  <si>
     <t>CodeableConcept.coding</t>
   </si>
   <si>
-    <t>union(., ./translation)</t>
-  </si>
-  <si>
-    <t>C*E.1-8, C*E.10-22</t>
-  </si>
-  <si>
-    <t>Procedure.code.coding.id</t>
-  </si>
-  <si>
-    <t>Procedure.code.coding.extension</t>
-  </si>
-  <si>
-    <t>Procedure.code.coding.system</t>
-  </si>
-  <si>
-    <t>Identity of the terminology system</t>
-  </si>
-  <si>
-    <t>The identification of the code system that defines the meaning of the symbol in the code.</t>
-  </si>
-  <si>
-    <t>The URI may be an OID (urn:oid:...) or a UUID (urn:uuid:...).  OIDs and UUIDs SHALL be references to the HL7 OID registry. Otherwise, the URI should come from HL7's list of FHIR defined special URIs or it should reference to some definition that establishes the system clearly and unambiguously.</t>
-  </si>
-  <si>
-    <t>Need to be unambiguous about the source of the definition of the symbol.</t>
-  </si>
-  <si>
-    <t>http://snomed.info/sct</t>
-  </si>
-  <si>
-    <t>Coding.system</t>
-  </si>
-  <si>
-    <t>./codeSystem</t>
-  </si>
-  <si>
-    <t>C*E.3</t>
-  </si>
-  <si>
-    <t>Procedure.code.coding.version</t>
-  </si>
-  <si>
-    <t>Version of the system - if relevant</t>
-  </si>
-  <si>
-    <t>The version of the code system which was used when choosing this code. Note that a well-maintained code system does not need the version reported, because the meaning of codes is consistent across versions. However this cannot consistently be assured, and when the meaning is not guaranteed to be consistent, the version SHOULD be exchanged.</t>
-  </si>
-  <si>
-    <t>Where the terminology does not clearly define what string should be used to identify code system versions, the recommendation is to use the date (expressed in FHIR date format) on which that version was officially published as the version date.</t>
-  </si>
-  <si>
-    <t>Coding.version</t>
-  </si>
-  <si>
-    <t>./codeSystemVersion</t>
-  </si>
-  <si>
-    <t>C*E.7</t>
-  </si>
-  <si>
-    <t>Procedure.code.coding.code</t>
-  </si>
-  <si>
-    <t>Symbol in syntax defined by the system</t>
-  </si>
-  <si>
-    <t>A symbol in syntax defined by the system. The symbol may be a predefined code or an expression in a syntax defined by the coding system (e.g. post-coordination).</t>
-  </si>
-  <si>
-    <t>Need to refer to a particular code in the system.</t>
-  </si>
-  <si>
-    <t>23426006</t>
-  </si>
-  <si>
-    <t>Coding.code</t>
-  </si>
-  <si>
-    <t>./code</t>
-  </si>
-  <si>
-    <t>C*E.1</t>
-  </si>
-  <si>
-    <t>Procedure.code.coding.display</t>
-  </si>
-  <si>
-    <t>Representation defined by the system</t>
-  </si>
-  <si>
-    <t>A representation of the meaning of the code in the system, following the rules of the system.</t>
-  </si>
-  <si>
-    <t>Need to be able to carry a human-readable meaning of the code for readers that do not know  the system.</t>
-  </si>
-  <si>
-    <t>Coding.display</t>
-  </si>
-  <si>
-    <t>CV.displayName</t>
-  </si>
-  <si>
-    <t>C*E.2 - but note this is not well followed</t>
-  </si>
-  <si>
-    <t>Procedure.code.coding.display.id</t>
-  </si>
-  <si>
-    <t>xml:id (or equivalent in JSON)</t>
-  </si>
-  <si>
-    <t>unique id for the element within a resource (for internal references)</t>
-  </si>
-  <si>
-    <t>Procedure.code.coding.display.extension</t>
-  </si>
-  <si>
-    <t>Procedure.code.coding.display.extension:translation</t>
-  </si>
-  <si>
-    <t>translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {translation}
-</t>
-  </si>
-  <si>
-    <t>Language Translation (Localization)</t>
-  </si>
-  <si>
-    <t>Language translation from base language of resource to another language.</t>
-  </si>
-  <si>
-    <t>ST.translation</t>
-  </si>
-  <si>
-    <t>Procedure.code.coding.display.value</t>
-  </si>
-  <si>
-    <t>Primitive value for string</t>
-  </si>
-  <si>
-    <t>The actual value</t>
-  </si>
-  <si>
-    <t>1048576</t>
-  </si>
-  <si>
-    <t>string.value</t>
-  </si>
-  <si>
-    <t>Procedure.code.coding.userSelected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boolean
-</t>
-  </si>
-  <si>
-    <t>If this coding was chosen directly by the user</t>
-  </si>
-  <si>
-    <t>Indicates that this coding was chosen by a user directly - e.g. off a pick list of available items (codes or displays).</t>
-  </si>
-  <si>
-    <t>Amongst a set of alternatives, a directly chosen code is the most appropriate starting point for new translations. There is some ambiguity about what exactly 'directly chosen' implies, and trading partner agreement may be needed to clarify the use of this element and its consequences more completely.</t>
-  </si>
-  <si>
-    <t>This has been identified as a clinical safety criterium - that this exact system/code pair was chosen explicitly, rather than inferred by the system based on some rules or language processing.</t>
-  </si>
-  <si>
-    <t>Coding.userSelected</t>
-  </si>
-  <si>
-    <t>CD.codingRationale</t>
-  </si>
-  <si>
-    <t>Sometimes implied by being first</t>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>CE/CNE/CWE subset one of the sets of component 1-3 or 4-6</t>
   </si>
   <si>
     <t>Procedure.code.text</t>
@@ -1032,6 +865,9 @@
   </si>
   <si>
     <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
+  </si>
+  <si>
+    <t>Mesure de la fonction respiratoire</t>
   </si>
   <si>
     <t>CodeableConcept.text</t>
@@ -2007,7 +1843,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN78"/>
+  <dimension ref="A1:AN67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -4734,7 +4570,7 @@
         <v>19</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>216</v>
+        <v>110</v>
       </c>
       <c r="Y24" s="2"/>
       <c r="Z24" t="s" s="2">
@@ -5034,7 +4870,7 @@
         <v>19</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K27" t="s" s="2">
         <v>257</v>
@@ -5059,7 +4895,7 @@
         <v>19</v>
       </c>
       <c r="S27" t="s" s="2">
-        <v>19</v>
+        <v>262</v>
       </c>
       <c r="T27" t="s" s="2">
         <v>19</v>
@@ -5098,7 +4934,7 @@
         <v>19</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>76</v>
@@ -5107,7 +4943,7 @@
         <v>77</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>19</v>
+        <v>148</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>97</v>
@@ -5116,21 +4952,21 @@
         <v>19</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -5144,25 +4980,29 @@
         <v>85</v>
       </c>
       <c r="H28" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="I28" t="s" s="2">
         <v>19</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="K28" t="s" s="2">
         <v>252</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>145</v>
+        <v>267</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
+        <v>268</v>
+      </c>
+      <c r="N28" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="O28" t="s" s="2">
+        <v>270</v>
+      </c>
       <c r="P28" t="s" s="2">
         <v>19</v>
       </c>
@@ -5171,7 +5011,7 @@
         <v>19</v>
       </c>
       <c r="S28" t="s" s="2">
-        <v>19</v>
+        <v>271</v>
       </c>
       <c r="T28" t="s" s="2">
         <v>19</v>
@@ -5210,7 +5050,7 @@
         <v>19</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>147</v>
+        <v>272</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>76</v>
@@ -5222,38 +5062,38 @@
         <v>19</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>149</v>
+        <v>273</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>19</v>
+        <v>274</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
-        <v>169</v>
+        <v>276</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>19</v>
@@ -5262,20 +5102,18 @@
         <v>19</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>131</v>
+        <v>277</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>172</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
         <v>19</v>
@@ -5312,51 +5150,51 @@
         <v>19</v>
       </c>
       <c r="AB29" t="s" s="2">
-        <v>134</v>
+        <v>19</v>
       </c>
       <c r="AC29" t="s" s="2">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="AD29" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>153</v>
+        <v>275</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>19</v>
+        <v>280</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>149</v>
+        <v>281</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>19</v>
+        <v>282</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>19</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>267</v>
+        <v>284</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>267</v>
+        <v>284</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5370,29 +5208,25 @@
         <v>85</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="I30" t="s" s="2">
         <v>19</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>99</v>
+        <v>252</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>268</v>
+        <v>145</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="O30" t="s" s="2">
-        <v>271</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
         <v>19</v>
       </c>
@@ -5401,7 +5235,7 @@
         <v>19</v>
       </c>
       <c r="S30" t="s" s="2">
-        <v>272</v>
+        <v>19</v>
       </c>
       <c r="T30" t="s" s="2">
         <v>19</v>
@@ -5440,7 +5274,7 @@
         <v>19</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>273</v>
+        <v>147</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>76</v>
@@ -5452,38 +5286,38 @@
         <v>19</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>274</v>
+        <v>149</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>275</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>19</v>
+        <v>169</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>19</v>
@@ -5492,19 +5326,19 @@
         <v>19</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>252</v>
+        <v>131</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>279</v>
+        <v>172</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -5542,51 +5376,51 @@
         <v>19</v>
       </c>
       <c r="AB31" t="s" s="2">
-        <v>19</v>
+        <v>134</v>
       </c>
       <c r="AC31" t="s" s="2">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="AD31" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>280</v>
+        <v>153</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI31" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>281</v>
+        <v>149</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>282</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5594,13 +5428,13 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>85</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="I32" t="s" s="2">
         <v>19</v>
@@ -5609,18 +5443,18 @@
         <v>86</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>105</v>
+        <v>252</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="N32" s="2"/>
-      <c r="O32" t="s" s="2">
-        <v>286</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
         <v>19</v>
       </c>
@@ -5629,7 +5463,7 @@
         <v>19</v>
       </c>
       <c r="S32" t="s" s="2">
-        <v>287</v>
+        <v>19</v>
       </c>
       <c r="T32" t="s" s="2">
         <v>19</v>
@@ -5668,7 +5502,7 @@
         <v>19</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>76</v>
@@ -5677,7 +5511,7 @@
         <v>85</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>19</v>
+        <v>291</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>97</v>
@@ -5686,21 +5520,21 @@
         <v>19</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>289</v>
+        <v>129</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>290</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5714,7 +5548,7 @@
         <v>85</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="I33" t="s" s="2">
         <v>19</v>
@@ -5723,18 +5557,18 @@
         <v>86</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>252</v>
+        <v>99</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="N33" s="2"/>
-      <c r="O33" t="s" s="2">
         <v>294</v>
       </c>
+      <c r="N33" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
         <v>19</v>
       </c>
@@ -5758,13 +5592,13 @@
         <v>19</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>19</v>
+        <v>296</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>19</v>
+        <v>297</v>
       </c>
       <c r="Z33" t="s" s="2">
-        <v>19</v>
+        <v>298</v>
       </c>
       <c r="AA33" t="s" s="2">
         <v>19</v>
@@ -5782,7 +5616,7 @@
         <v>19</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>76</v>
@@ -5800,21 +5634,21 @@
         <v>19</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>296</v>
+        <v>129</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>297</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5834,18 +5668,20 @@
         <v>19</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>252</v>
+        <v>176</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="N34" s="2"/>
+        <v>302</v>
+      </c>
+      <c r="N34" t="s" s="2">
+        <v>303</v>
+      </c>
       <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
         <v>19</v>
@@ -5894,7 +5730,7 @@
         <v>19</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>147</v>
+        <v>304</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>76</v>
@@ -5906,13 +5742,13 @@
         <v>19</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>19</v>
+        <v>305</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>19</v>
@@ -5923,10 +5759,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5937,7 +5773,7 @@
         <v>76</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>19</v>
@@ -5946,18 +5782,20 @@
         <v>19</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>131</v>
+        <v>252</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>132</v>
+        <v>307</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="N35" s="2"/>
+        <v>308</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>309</v>
+      </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
         <v>19</v>
@@ -5994,35 +5832,37 @@
         <v>19</v>
       </c>
       <c r="AB35" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="AC35" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="AC35" t="s" s="2">
+        <v>19</v>
+      </c>
       <c r="AD35" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>153</v>
+        <v>310</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>19</v>
@@ -6033,14 +5873,12 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="C36" t="s" s="2">
-        <v>303</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
         <v>19</v>
       </c>
@@ -6049,7 +5887,7 @@
         <v>76</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>19</v>
@@ -6058,18 +5896,20 @@
         <v>19</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="N36" s="2"/>
+        <v>314</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>315</v>
+      </c>
       <c r="O36" s="2"/>
       <c r="P36" t="s" s="2">
         <v>19</v>
@@ -6118,39 +5958,39 @@
         <v>19</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>153</v>
+        <v>311</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>19</v>
+        <v>316</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>19</v>
+        <v>318</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>19</v>
+        <v>319</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6158,7 +5998,7 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>85</v>
@@ -6170,18 +6010,20 @@
         <v>19</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>252</v>
+        <v>321</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="N37" s="2"/>
+        <v>323</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>324</v>
+      </c>
       <c r="O37" s="2"/>
       <c r="P37" t="s" s="2">
         <v>19</v>
@@ -6203,7 +6045,7 @@
         <v>19</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>311</v>
+        <v>19</v>
       </c>
       <c r="X37" t="s" s="2">
         <v>19</v>
@@ -6230,7 +6072,7 @@
         <v>19</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>76</v>
@@ -6242,27 +6084,27 @@
         <v>19</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>19</v>
+        <v>325</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>19</v>
+        <v>326</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>19</v>
+        <v>327</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>19</v>
+        <v>328</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>313</v>
+        <v>329</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>313</v>
+        <v>329</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6282,23 +6124,19 @@
         <v>19</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>314</v>
+        <v>252</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>315</v>
+        <v>145</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>318</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
         <v>19</v>
       </c>
@@ -6346,7 +6184,7 @@
         <v>19</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>319</v>
+        <v>147</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>76</v>
@@ -6358,63 +6196,61 @@
         <v>19</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>320</v>
+        <v>149</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>321</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>19</v>
+        <v>169</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H39" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="I39" t="s" s="2">
         <v>19</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>252</v>
+        <v>131</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>323</v>
+        <v>254</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>324</v>
+        <v>255</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="O39" t="s" s="2">
-        <v>326</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
         <v>19</v>
       </c>
@@ -6450,59 +6286,61 @@
         <v>19</v>
       </c>
       <c r="AB39" t="s" s="2">
-        <v>19</v>
+        <v>134</v>
       </c>
       <c r="AC39" t="s" s="2">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="AD39" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>327</v>
+        <v>153</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>328</v>
+        <v>149</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>329</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B40" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="C40" s="2"/>
+      <c r="C40" t="s" s="2">
+        <v>332</v>
+      </c>
       <c r="D40" t="s" s="2">
-        <v>331</v>
+        <v>19</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>85</v>
@@ -6514,16 +6352,16 @@
         <v>19</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6574,39 +6412,39 @@
         <v>19</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>330</v>
+        <v>153</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>335</v>
+        <v>19</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>336</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>337</v>
+        <v>19</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>338</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6626,16 +6464,16 @@
         <v>19</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>252</v>
+        <v>338</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>145</v>
+        <v>339</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>146</v>
+        <v>340</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6686,7 +6524,7 @@
         <v>19</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>147</v>
+        <v>337</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>76</v>
@@ -6698,16 +6536,16 @@
         <v>19</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>149</v>
+        <v>341</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>19</v>
+        <v>342</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>19</v>
@@ -6715,21 +6553,21 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>19</v>
@@ -6738,20 +6576,18 @@
         <v>19</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>131</v>
+        <v>338</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>254</v>
+        <v>344</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>172</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
         <v>19</v>
@@ -6788,40 +6624,40 @@
         <v>19</v>
       </c>
       <c r="AB42" t="s" s="2">
-        <v>134</v>
+        <v>19</v>
       </c>
       <c r="AC42" t="s" s="2">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="AD42" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>153</v>
+        <v>343</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>149</v>
+        <v>346</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>19</v>
+        <v>347</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>19</v>
@@ -6829,10 +6665,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6840,10 +6676,10 @@
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>19</v>
@@ -6855,17 +6691,15 @@
         <v>86</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>252</v>
+        <v>349</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>344</v>
-      </c>
+        <v>351</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
         <v>19</v>
@@ -6914,25 +6748,25 @@
         <v>19</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>346</v>
+        <v>19</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>97</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>19</v>
+        <v>352</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>129</v>
+        <v>353</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>19</v>
@@ -6943,10 +6777,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6966,20 +6800,18 @@
         <v>19</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>99</v>
+        <v>252</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>348</v>
+        <v>145</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>349</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>350</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
         <v>19</v>
@@ -7004,13 +6836,13 @@
         <v>19</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>351</v>
+        <v>19</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>352</v>
+        <v>19</v>
       </c>
       <c r="Z44" t="s" s="2">
-        <v>353</v>
+        <v>19</v>
       </c>
       <c r="AA44" t="s" s="2">
         <v>19</v>
@@ -7028,7 +6860,7 @@
         <v>19</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>354</v>
+        <v>147</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>76</v>
@@ -7040,13 +6872,13 @@
         <v>19</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>19</v>
@@ -7064,14 +6896,14 @@
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>19</v>
+        <v>169</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>19</v>
@@ -7080,19 +6912,19 @@
         <v>19</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>176</v>
+        <v>131</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>356</v>
+        <v>254</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>357</v>
+        <v>255</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>358</v>
+        <v>172</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -7142,25 +6974,25 @@
         <v>19</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>359</v>
+        <v>153</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>360</v>
+        <v>149</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>19</v>
@@ -7171,44 +7003,46 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>19</v>
+        <v>357</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>19</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="J46" t="s" s="2">
         <v>86</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>252</v>
+        <v>131</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="O46" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="O46" t="s" s="2">
+        <v>173</v>
+      </c>
       <c r="P46" t="s" s="2">
         <v>19</v>
       </c>
@@ -7256,19 +7090,19 @@
         <v>19</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>19</v>
@@ -7285,10 +7119,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7311,18 +7145,18 @@
         <v>86</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>367</v>
+        <v>224</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="O47" s="2"/>
+        <v>363</v>
+      </c>
+      <c r="N47" s="2"/>
+      <c r="O47" t="s" s="2">
+        <v>364</v>
+      </c>
       <c r="P47" t="s" s="2">
         <v>19</v>
       </c>
@@ -7346,13 +7180,13 @@
         <v>19</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>19</v>
+        <v>365</v>
       </c>
       <c r="Z47" t="s" s="2">
-        <v>19</v>
+        <v>366</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>19</v>
@@ -7370,7 +7204,7 @@
         <v>19</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>76</v>
@@ -7385,24 +7219,24 @@
         <v>97</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>373</v>
+        <v>19</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7425,18 +7259,18 @@
         <v>86</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="O48" s="2"/>
+        <v>373</v>
+      </c>
+      <c r="N48" s="2"/>
+      <c r="O48" t="s" s="2">
+        <v>374</v>
+      </c>
       <c r="P48" t="s" s="2">
         <v>19</v>
       </c>
@@ -7484,10 +7318,10 @@
         <v>19</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>85</v>
@@ -7499,24 +7333,24 @@
         <v>97</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7539,16 +7373,18 @@
         <v>19</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>252</v>
+        <v>380</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>145</v>
+        <v>381</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>146</v>
+        <v>382</v>
       </c>
       <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
+      <c r="O49" t="s" s="2">
+        <v>383</v>
+      </c>
       <c r="P49" t="s" s="2">
         <v>19</v>
       </c>
@@ -7596,7 +7432,7 @@
         <v>19</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>147</v>
+        <v>379</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>76</v>
@@ -7608,13 +7444,13 @@
         <v>19</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>149</v>
+        <v>384</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>19</v>
@@ -7632,14 +7468,14 @@
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
         <v>76</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>19</v>
@@ -7648,21 +7484,21 @@
         <v>19</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>131</v>
+        <v>386</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>254</v>
+        <v>387</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="O50" s="2"/>
+        <v>388</v>
+      </c>
+      <c r="N50" s="2"/>
+      <c r="O50" t="s" s="2">
+        <v>389</v>
+      </c>
       <c r="P50" t="s" s="2">
         <v>19</v>
       </c>
@@ -7698,40 +7534,40 @@
         <v>19</v>
       </c>
       <c r="AB50" t="s" s="2">
-        <v>134</v>
+        <v>19</v>
       </c>
       <c r="AC50" t="s" s="2">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="AD50" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>153</v>
+        <v>385</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>149</v>
+        <v>390</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>19</v>
+        <v>391</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>19</v>
@@ -7739,14 +7575,12 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="C51" t="s" s="2">
-        <v>387</v>
-      </c>
+        <v>392</v>
+      </c>
+      <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
         <v>19</v>
       </c>
@@ -7755,7 +7589,7 @@
         <v>76</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>19</v>
@@ -7764,18 +7598,20 @@
         <v>19</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>388</v>
+        <v>224</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="N51" s="2"/>
+        <v>394</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>395</v>
+      </c>
       <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
         <v>19</v>
@@ -7800,13 +7636,13 @@
         <v>19</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>19</v>
+        <v>396</v>
       </c>
       <c r="Z51" t="s" s="2">
-        <v>19</v>
+        <v>397</v>
       </c>
       <c r="AA51" t="s" s="2">
         <v>19</v>
@@ -7824,7 +7660,7 @@
         <v>19</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>153</v>
+        <v>392</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>76</v>
@@ -7836,16 +7672,16 @@
         <v>19</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>19</v>
+        <v>398</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>19</v>
+        <v>400</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>19</v>
@@ -7853,10 +7689,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7867,7 +7703,7 @@
         <v>76</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>19</v>
@@ -7879,15 +7715,17 @@
         <v>86</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="N52" s="2"/>
+        <v>404</v>
+      </c>
+      <c r="N52" t="s" s="2">
+        <v>405</v>
+      </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
         <v>19</v>
@@ -7936,13 +7774,13 @@
         <v>19</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>19</v>
@@ -7951,13 +7789,13 @@
         <v>97</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>19</v>
+        <v>406</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>19</v>
@@ -7965,10 +7803,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7979,7 +7817,7 @@
         <v>76</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H53" t="s" s="2">
         <v>19</v>
@@ -7991,15 +7829,17 @@
         <v>86</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>393</v>
+        <v>242</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>400</v>
-      </c>
-      <c r="N53" s="2"/>
+        <v>409</v>
+      </c>
+      <c r="N53" t="s" s="2">
+        <v>410</v>
+      </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
         <v>19</v>
@@ -8024,13 +7864,11 @@
         <v>19</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y53" t="s" s="2">
-        <v>19</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="Y53" s="2"/>
       <c r="Z53" t="s" s="2">
-        <v>19</v>
+        <v>411</v>
       </c>
       <c r="AA53" t="s" s="2">
         <v>19</v>
@@ -8048,13 +7886,13 @@
         <v>19</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH53" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI53" t="s" s="2">
         <v>19</v>
@@ -8066,21 +7904,21 @@
         <v>19</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>402</v>
+        <v>19</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>19</v>
+        <v>413</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8091,7 +7929,7 @@
         <v>76</v>
       </c>
       <c r="G54" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H54" t="s" s="2">
         <v>19</v>
@@ -8103,15 +7941,17 @@
         <v>86</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>404</v>
+        <v>224</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>406</v>
-      </c>
-      <c r="N54" s="2"/>
+        <v>416</v>
+      </c>
+      <c r="N54" t="s" s="2">
+        <v>417</v>
+      </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
         <v>19</v>
@@ -8136,13 +7976,13 @@
         <v>19</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>19</v>
+        <v>418</v>
       </c>
       <c r="Z54" t="s" s="2">
-        <v>19</v>
+        <v>419</v>
       </c>
       <c r="AA54" t="s" s="2">
         <v>19</v>
@@ -8160,13 +8000,13 @@
         <v>19</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH54" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI54" t="s" s="2">
         <v>19</v>
@@ -8175,10 +8015,10 @@
         <v>97</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>407</v>
+        <v>19</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>19</v>
@@ -8189,10 +8029,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>409</v>
+        <v>421</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>409</v>
+        <v>421</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8203,7 +8043,7 @@
         <v>76</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>19</v>
@@ -8215,15 +8055,17 @@
         <v>19</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>252</v>
+        <v>422</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>145</v>
+        <v>423</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="N55" s="2"/>
+        <v>424</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>425</v>
+      </c>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
         <v>19</v>
@@ -8272,25 +8114,25 @@
         <v>19</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>147</v>
+        <v>421</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>149</v>
+        <v>426</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>19</v>
@@ -8301,14 +8143,14 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>410</v>
+        <v>427</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>410</v>
+        <v>427</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
@@ -8327,16 +8169,16 @@
         <v>19</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>131</v>
+        <v>224</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>254</v>
+        <v>428</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>255</v>
+        <v>429</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>172</v>
+        <v>430</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
@@ -8362,13 +8204,13 @@
         <v>19</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>19</v>
+        <v>431</v>
       </c>
       <c r="Z56" t="s" s="2">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="AA56" t="s" s="2">
         <v>19</v>
@@ -8386,7 +8228,7 @@
         <v>19</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>153</v>
+        <v>427</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>76</v>
@@ -8398,13 +8240,13 @@
         <v>19</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="AK56" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>149</v>
+        <v>433</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>19</v>
@@ -8415,14 +8257,14 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>411</v>
+        <v>434</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>411</v>
+        <v>434</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
-        <v>412</v>
+        <v>19</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
@@ -8435,25 +8277,23 @@
         <v>19</v>
       </c>
       <c r="I57" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>131</v>
+        <v>435</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>413</v>
+        <v>436</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>414</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>172</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
-        <v>173</v>
+        <v>438</v>
       </c>
       <c r="P57" t="s" s="2">
         <v>19</v>
@@ -8502,7 +8342,7 @@
         <v>19</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>415</v>
+        <v>434</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>76</v>
@@ -8514,13 +8354,13 @@
         <v>19</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="AK57" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>129</v>
+        <v>433</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>19</v>
@@ -8531,10 +8371,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>416</v>
+        <v>439</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>416</v>
+        <v>439</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8545,7 +8385,7 @@
         <v>76</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>19</v>
@@ -8554,21 +8394,19 @@
         <v>19</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K58" t="s" s="2">
         <v>224</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>417</v>
+        <v>440</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>418</v>
+        <v>441</v>
       </c>
       <c r="N58" s="2"/>
-      <c r="O58" t="s" s="2">
-        <v>419</v>
-      </c>
+      <c r="O58" s="2"/>
       <c r="P58" t="s" s="2">
         <v>19</v>
       </c>
@@ -8595,10 +8433,10 @@
         <v>228</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>420</v>
+        <v>442</v>
       </c>
       <c r="Z58" t="s" s="2">
-        <v>421</v>
+        <v>443</v>
       </c>
       <c r="AA58" t="s" s="2">
         <v>19</v>
@@ -8616,13 +8454,13 @@
         <v>19</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>416</v>
+        <v>439</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>19</v>
@@ -8631,24 +8469,24 @@
         <v>97</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>422</v>
+        <v>19</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>423</v>
+        <v>444</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>424</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>425</v>
+        <v>445</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>425</v>
+        <v>445</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8656,10 +8494,10 @@
       </c>
       <c r="E59" s="2"/>
       <c r="F59" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>19</v>
@@ -8668,21 +8506,19 @@
         <v>19</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>426</v>
+        <v>446</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>427</v>
+        <v>447</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>428</v>
+        <v>448</v>
       </c>
       <c r="N59" s="2"/>
-      <c r="O59" t="s" s="2">
-        <v>429</v>
-      </c>
+      <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
         <v>19</v>
       </c>
@@ -8730,13 +8566,13 @@
         <v>19</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>425</v>
+        <v>445</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>19</v>
@@ -8745,24 +8581,24 @@
         <v>97</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>430</v>
+        <v>449</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>431</v>
+        <v>450</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>432</v>
+        <v>19</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>433</v>
+        <v>451</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>434</v>
+        <v>452</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>434</v>
+        <v>452</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8773,7 +8609,7 @@
         <v>76</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H60" t="s" s="2">
         <v>19</v>
@@ -8785,18 +8621,16 @@
         <v>19</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>435</v>
+        <v>349</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>436</v>
+        <v>453</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>437</v>
+        <v>454</v>
       </c>
       <c r="N60" s="2"/>
-      <c r="O60" t="s" s="2">
-        <v>438</v>
-      </c>
+      <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
         <v>19</v>
       </c>
@@ -8844,13 +8678,13 @@
         <v>19</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>434</v>
+        <v>452</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH60" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AI60" t="s" s="2">
         <v>19</v>
@@ -8862,7 +8696,7 @@
         <v>19</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>439</v>
+        <v>455</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>19</v>
@@ -8873,10 +8707,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>440</v>
+        <v>456</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>440</v>
+        <v>456</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8896,21 +8730,19 @@
         <v>19</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>441</v>
+        <v>252</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>442</v>
+        <v>145</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>443</v>
+        <v>146</v>
       </c>
       <c r="N61" s="2"/>
-      <c r="O61" t="s" s="2">
-        <v>444</v>
-      </c>
+      <c r="O61" s="2"/>
       <c r="P61" t="s" s="2">
         <v>19</v>
       </c>
@@ -8958,7 +8790,7 @@
         <v>19</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>440</v>
+        <v>147</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>76</v>
@@ -8970,16 +8802,16 @@
         <v>19</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>445</v>
+        <v>149</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>446</v>
+        <v>19</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>19</v>
@@ -8987,14 +8819,14 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
-        <v>19</v>
+        <v>169</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
@@ -9010,19 +8842,19 @@
         <v>19</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>224</v>
+        <v>131</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>448</v>
+        <v>254</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>449</v>
+        <v>255</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>450</v>
+        <v>172</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
@@ -9048,13 +8880,13 @@
         <v>19</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>228</v>
+        <v>19</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>451</v>
+        <v>19</v>
       </c>
       <c r="Z62" t="s" s="2">
-        <v>452</v>
+        <v>19</v>
       </c>
       <c r="AA62" t="s" s="2">
         <v>19</v>
@@ -9072,7 +8904,7 @@
         <v>19</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>447</v>
+        <v>153</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>76</v>
@@ -9084,16 +8916,16 @@
         <v>19</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>453</v>
+        <v>19</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>454</v>
+        <v>149</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>455</v>
+        <v>19</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>19</v>
@@ -9101,14 +8933,14 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
-        <v>19</v>
+        <v>357</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" t="s" s="2">
@@ -9121,24 +8953,26 @@
         <v>19</v>
       </c>
       <c r="I63" t="s" s="2">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="J63" t="s" s="2">
         <v>86</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>457</v>
+        <v>131</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>458</v>
+        <v>358</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>459</v>
+        <v>359</v>
       </c>
       <c r="N63" t="s" s="2">
-        <v>460</v>
-      </c>
-      <c r="O63" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="O63" t="s" s="2">
+        <v>173</v>
+      </c>
       <c r="P63" t="s" s="2">
         <v>19</v>
       </c>
@@ -9186,7 +9020,7 @@
         <v>19</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>456</v>
+        <v>360</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>76</v>
@@ -9198,16 +9032,16 @@
         <v>19</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>461</v>
+        <v>19</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>454</v>
+        <v>129</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>455</v>
+        <v>19</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>19</v>
@@ -9215,10 +9049,10 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9229,7 +9063,7 @@
         <v>76</v>
       </c>
       <c r="G64" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H64" t="s" s="2">
         <v>19</v>
@@ -9238,20 +9072,18 @@
         <v>19</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>464</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>465</v>
-      </c>
+        <v>461</v>
+      </c>
+      <c r="N64" s="2"/>
       <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
         <v>19</v>
@@ -9278,9 +9110,11 @@
       <c r="X64" t="s" s="2">
         <v>110</v>
       </c>
-      <c r="Y64" s="2"/>
+      <c r="Y64" t="s" s="2">
+        <v>462</v>
+      </c>
       <c r="Z64" t="s" s="2">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="AA64" t="s" s="2">
         <v>19</v>
@@ -9298,13 +9132,13 @@
         <v>19</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AI64" t="s" s="2">
         <v>19</v>
@@ -9316,21 +9150,21 @@
         <v>19</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="AM64" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN64" t="s" s="2">
-        <v>468</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9338,7 +9172,7 @@
       </c>
       <c r="E65" s="2"/>
       <c r="F65" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G65" t="s" s="2">
         <v>85</v>
@@ -9350,20 +9184,18 @@
         <v>19</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>224</v>
+        <v>466</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>471</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>472</v>
-      </c>
+        <v>468</v>
+      </c>
+      <c r="N65" s="2"/>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
         <v>19</v>
@@ -9388,13 +9220,13 @@
         <v>19</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>228</v>
+        <v>19</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>473</v>
+        <v>19</v>
       </c>
       <c r="Z65" t="s" s="2">
-        <v>474</v>
+        <v>19</v>
       </c>
       <c r="AA65" t="s" s="2">
         <v>19</v>
@@ -9412,10 +9244,10 @@
         <v>19</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="AH65" t="s" s="2">
         <v>85</v>
@@ -9430,7 +9262,7 @@
         <v>19</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>19</v>
@@ -9441,10 +9273,10 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9467,18 +9299,20 @@
         <v>19</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>480</v>
-      </c>
-      <c r="O66" s="2"/>
+        <v>474</v>
+      </c>
+      <c r="O66" t="s" s="2">
+        <v>475</v>
+      </c>
       <c r="P66" t="s" s="2">
         <v>19</v>
       </c>
@@ -9526,7 +9360,7 @@
         <v>19</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>76</v>
@@ -9544,7 +9378,7 @@
         <v>19</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>19</v>
@@ -9555,10 +9389,10 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -9584,13 +9418,13 @@
         <v>224</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>485</v>
+        <v>474</v>
       </c>
       <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
@@ -9619,10 +9453,10 @@
         <v>228</v>
       </c>
       <c r="Y67" t="s" s="2">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="Z67" t="s" s="2">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="AA67" t="s" s="2">
         <v>19</v>
@@ -9640,7 +9474,7 @@
         <v>19</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>76</v>
@@ -9658,1263 +9492,17 @@
         <v>19</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AN67" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="68" hidden="true">
-      <c r="A68" t="s" s="2">
-        <v>489</v>
-      </c>
-      <c r="B68" t="s" s="2">
-        <v>489</v>
-      </c>
-      <c r="C68" s="2"/>
-      <c r="D68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E68" s="2"/>
-      <c r="F68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="G68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K68" t="s" s="2">
-        <v>490</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>491</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>492</v>
-      </c>
-      <c r="N68" s="2"/>
-      <c r="O68" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="P68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q68" s="2"/>
-      <c r="R68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF68" t="s" s="2">
-        <v>489</v>
-      </c>
-      <c r="AG68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AI68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ68" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AK68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AL68" t="s" s="2">
-        <v>488</v>
-      </c>
-      <c r="AM68" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AN68" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="69" hidden="true">
-      <c r="A69" t="s" s="2">
-        <v>494</v>
-      </c>
-      <c r="B69" t="s" s="2">
-        <v>494</v>
-      </c>
-      <c r="C69" s="2"/>
-      <c r="D69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E69" s="2"/>
-      <c r="F69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="G69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K69" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="L69" t="s" s="2">
-        <v>495</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>496</v>
-      </c>
-      <c r="N69" s="2"/>
-      <c r="O69" s="2"/>
-      <c r="P69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q69" s="2"/>
-      <c r="R69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X69" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="Y69" t="s" s="2">
-        <v>497</v>
-      </c>
-      <c r="Z69" t="s" s="2">
-        <v>498</v>
-      </c>
-      <c r="AA69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF69" t="s" s="2">
-        <v>494</v>
-      </c>
-      <c r="AG69" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AI69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ69" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AK69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AL69" t="s" s="2">
-        <v>499</v>
-      </c>
-      <c r="AM69" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AN69" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="70" hidden="true">
-      <c r="A70" t="s" s="2">
-        <v>500</v>
-      </c>
-      <c r="B70" t="s" s="2">
-        <v>500</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E70" s="2"/>
-      <c r="F70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="G70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K70" t="s" s="2">
-        <v>501</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>502</v>
-      </c>
-      <c r="M70" t="s" s="2">
-        <v>503</v>
-      </c>
-      <c r="N70" s="2"/>
-      <c r="O70" s="2"/>
-      <c r="P70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q70" s="2"/>
-      <c r="R70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF70" t="s" s="2">
-        <v>500</v>
-      </c>
-      <c r="AG70" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AI70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ70" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AK70" t="s" s="2">
-        <v>504</v>
-      </c>
-      <c r="AL70" t="s" s="2">
-        <v>505</v>
-      </c>
-      <c r="AM70" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AN70" t="s" s="2">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="71" hidden="true">
-      <c r="A71" t="s" s="2">
-        <v>507</v>
-      </c>
-      <c r="B71" t="s" s="2">
-        <v>507</v>
-      </c>
-      <c r="C71" s="2"/>
-      <c r="D71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E71" s="2"/>
-      <c r="F71" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="G71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K71" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="L71" t="s" s="2">
-        <v>508</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>509</v>
-      </c>
-      <c r="N71" s="2"/>
-      <c r="O71" s="2"/>
-      <c r="P71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q71" s="2"/>
-      <c r="R71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF71" t="s" s="2">
-        <v>507</v>
-      </c>
-      <c r="AG71" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AI71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ71" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AK71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AL71" t="s" s="2">
-        <v>510</v>
-      </c>
-      <c r="AM71" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AN71" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="72" hidden="true">
-      <c r="A72" t="s" s="2">
-        <v>511</v>
-      </c>
-      <c r="B72" t="s" s="2">
-        <v>511</v>
-      </c>
-      <c r="C72" s="2"/>
-      <c r="D72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E72" s="2"/>
-      <c r="F72" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="G72" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="H72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K72" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="N72" s="2"/>
-      <c r="O72" s="2"/>
-      <c r="P72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q72" s="2"/>
-      <c r="R72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF72" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="AG72" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH72" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="AI72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AK72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AL72" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="AM72" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AN72" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="73" hidden="true">
-      <c r="A73" t="s" s="2">
-        <v>512</v>
-      </c>
-      <c r="B73" t="s" s="2">
-        <v>512</v>
-      </c>
-      <c r="C73" s="2"/>
-      <c r="D73" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="E73" s="2"/>
-      <c r="F73" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="G73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K73" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="N73" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="O73" s="2"/>
-      <c r="P73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q73" s="2"/>
-      <c r="R73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF73" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="AG73" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AI73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ73" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="AK73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AL73" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="AM73" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AN73" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="74" hidden="true">
-      <c r="A74" t="s" s="2">
-        <v>513</v>
-      </c>
-      <c r="B74" t="s" s="2">
-        <v>513</v>
-      </c>
-      <c r="C74" s="2"/>
-      <c r="D74" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="E74" s="2"/>
-      <c r="F74" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="G74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I74" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="J74" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="K74" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>414</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="O74" t="s" s="2">
-        <v>173</v>
-      </c>
-      <c r="P74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q74" s="2"/>
-      <c r="R74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF74" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="AG74" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AI74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="AK74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AL74" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="AM74" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AN74" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" hidden="true">
-      <c r="A75" t="s" s="2">
-        <v>514</v>
-      </c>
-      <c r="B75" t="s" s="2">
-        <v>514</v>
-      </c>
-      <c r="C75" s="2"/>
-      <c r="D75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E75" s="2"/>
-      <c r="F75" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="G75" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="H75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K75" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="L75" t="s" s="2">
-        <v>515</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>516</v>
-      </c>
-      <c r="N75" s="2"/>
-      <c r="O75" s="2"/>
-      <c r="P75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q75" s="2"/>
-      <c r="R75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X75" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="Y75" t="s" s="2">
-        <v>517</v>
-      </c>
-      <c r="Z75" t="s" s="2">
-        <v>518</v>
-      </c>
-      <c r="AA75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF75" t="s" s="2">
-        <v>514</v>
-      </c>
-      <c r="AG75" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH75" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="AI75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ75" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AK75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AL75" t="s" s="2">
-        <v>519</v>
-      </c>
-      <c r="AM75" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AN75" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="76" hidden="true">
-      <c r="A76" t="s" s="2">
-        <v>520</v>
-      </c>
-      <c r="B76" t="s" s="2">
-        <v>520</v>
-      </c>
-      <c r="C76" s="2"/>
-      <c r="D76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E76" s="2"/>
-      <c r="F76" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="G76" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="H76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K76" t="s" s="2">
-        <v>521</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>522</v>
-      </c>
-      <c r="M76" t="s" s="2">
-        <v>523</v>
-      </c>
-      <c r="N76" s="2"/>
-      <c r="O76" s="2"/>
-      <c r="P76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q76" s="2"/>
-      <c r="R76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF76" t="s" s="2">
-        <v>520</v>
-      </c>
-      <c r="AG76" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="AH76" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="AI76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ76" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AK76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>524</v>
-      </c>
-      <c r="AM76" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AN76" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="77" hidden="true">
-      <c r="A77" t="s" s="2">
-        <v>525</v>
-      </c>
-      <c r="B77" t="s" s="2">
-        <v>525</v>
-      </c>
-      <c r="C77" s="2"/>
-      <c r="D77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E77" s="2"/>
-      <c r="F77" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="G77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K77" t="s" s="2">
-        <v>526</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>527</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>528</v>
-      </c>
-      <c r="N77" t="s" s="2">
-        <v>529</v>
-      </c>
-      <c r="O77" t="s" s="2">
-        <v>530</v>
-      </c>
-      <c r="P77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q77" s="2"/>
-      <c r="R77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Y77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF77" t="s" s="2">
-        <v>525</v>
-      </c>
-      <c r="AG77" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AI77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ77" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AK77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AL77" t="s" s="2">
-        <v>531</v>
-      </c>
-      <c r="AM77" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AN77" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="78" hidden="true">
-      <c r="A78" t="s" s="2">
-        <v>532</v>
-      </c>
-      <c r="B78" t="s" s="2">
-        <v>532</v>
-      </c>
-      <c r="C78" s="2"/>
-      <c r="D78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="E78" s="2"/>
-      <c r="F78" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="G78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="I78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="K78" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>533</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>534</v>
-      </c>
-      <c r="N78" t="s" s="2">
-        <v>529</v>
-      </c>
-      <c r="O78" s="2"/>
-      <c r="P78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q78" s="2"/>
-      <c r="R78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="S78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="T78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="U78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="V78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="W78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="X78" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="Y78" t="s" s="2">
-        <v>535</v>
-      </c>
-      <c r="Z78" t="s" s="2">
-        <v>536</v>
-      </c>
-      <c r="AA78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AB78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AC78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AD78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AE78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AF78" t="s" s="2">
-        <v>532</v>
-      </c>
-      <c r="AG78" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AI78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AJ78" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AK78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AL78" t="s" s="2">
-        <v>537</v>
-      </c>
-      <c r="AM78" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="AN78" t="s" s="2">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN78">
+  <autoFilter ref="A1:AN67">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10924,7 +9512,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI77">
+  <conditionalFormatting sqref="A2:AI66">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>